<commit_message>
feat: added shapes and device settings
</commit_message>
<xml_diff>
--- a/protocol.xlsx
+++ b/protocol.xlsx
@@ -391,7 +391,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +403,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF00b050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -544,71 +550,71 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,11 +924,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="23" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="24" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="23" width="31.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="23" width="32.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="23" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="22" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="23" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="24" width="31.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="24" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="24" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
@@ -1440,46 +1446,46 @@
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="16.5">
       <c r="A36" s="3"/>
-      <c r="B36" s="10"/>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="16.5">
       <c r="A37" s="3"/>
-      <c r="B37" s="10"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="16.5">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="13" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="16.5">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="13">
         <v>1</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="14">
         <v>1</v>
       </c>
       <c r="E39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="16.5">
-      <c r="A40" s="13"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
@@ -1490,7 +1496,7 @@
       <c r="E40" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="16.5">
-      <c r="A41" s="13"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="5" t="s">
         <v>47</v>
       </c>
@@ -1503,7 +1509,7 @@
       <c r="E41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="16.5">
-      <c r="A42" s="13"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
@@ -1516,7 +1522,7 @@
       <c r="E42" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
-      <c r="A43" s="13"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1529,18 +1535,18 @@
       <c r="E43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="16.5">
-      <c r="A44" s="13"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="13"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="4"/>
       <c r="E44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="16.5">
-      <c r="A45" s="13"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="12"/>
+      <c r="B45" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D45" s="4">
@@ -1549,11 +1555,11 @@
       <c r="E45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="16.5">
-      <c r="A46" s="13"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="12"/>
+      <c r="B46" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>53</v>
       </c>
       <c r="D46" s="4">
@@ -1562,7 +1568,7 @@
       <c r="E46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="16.5">
-      <c r="A47" s="13"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="5" t="s">
         <v>54</v>
       </c>
@@ -1575,25 +1581,25 @@
       <c r="E47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="16.5">
-      <c r="A48" s="13"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
       <c r="E48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="16.5">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
       <c r="E49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="16.5">
-      <c r="A50" s="11"/>
+      <c r="A50" s="10"/>
       <c r="B50" s="5" t="s">
         <v>58</v>
       </c>
@@ -1601,25 +1607,25 @@
       <c r="D50" s="4">
         <v>1</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="16.5">
-      <c r="A51" s="13"/>
-      <c r="B51" s="12" t="s">
+      <c r="A51" s="12"/>
+      <c r="B51" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="14"/>
+      <c r="C51" s="13"/>
       <c r="D51" s="4">
         <v>2</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="16.5">
-      <c r="A52" s="13"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="5" t="s">
         <v>62</v>
       </c>
@@ -1627,12 +1633,12 @@
       <c r="D52" s="4">
         <v>4</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="16.5">
-      <c r="A53" s="13"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="5" t="s">
         <v>64</v>
       </c>
@@ -1640,12 +1646,12 @@
       <c r="D53" s="4">
         <v>8</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="16.5">
-      <c r="A54" s="13"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="5" t="s">
         <v>66</v>
       </c>
@@ -1653,12 +1659,12 @@
       <c r="D54" s="4">
         <v>1</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="16.5">
-      <c r="A55" s="13"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="5" t="s">
         <v>68</v>
       </c>
@@ -1666,12 +1672,12 @@
       <c r="D55" s="4">
         <v>2</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="15" t="s">
         <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="16.5">
-      <c r="A56" s="13"/>
+      <c r="A56" s="12"/>
       <c r="B56" s="5" t="s">
         <v>70</v>
       </c>
@@ -1679,12 +1685,12 @@
       <c r="D56" s="4">
         <v>4</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>71</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="16.5">
-      <c r="A57" s="11"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="5" t="s">
         <v>72</v>
       </c>
@@ -1692,12 +1698,12 @@
       <c r="D57" s="4">
         <v>8</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>73</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="16.5">
-      <c r="A58" s="13"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="5" t="s">
         <v>74</v>
       </c>
@@ -1705,46 +1711,46 @@
       <c r="D58" s="4">
         <v>1</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="16.5">
-      <c r="A59" s="13"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="5"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="16.5">
-      <c r="A60" s="13"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
       <c r="E60" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="16.5">
-      <c r="A61" s="13"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
       <c r="E61" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="16.5">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="13"/>
+      <c r="D62" s="12"/>
       <c r="E62" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="16.5">
-      <c r="A63" s="13"/>
+      <c r="A63" s="12"/>
       <c r="B63" s="5">
         <v>1200</v>
       </c>
@@ -1757,7 +1763,7 @@
       <c r="E63" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="16.5">
-      <c r="A64" s="13"/>
+      <c r="A64" s="12"/>
       <c r="B64" s="5">
         <v>2400</v>
       </c>
@@ -1770,7 +1776,7 @@
       <c r="E64" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="16.5">
-      <c r="A65" s="13"/>
+      <c r="A65" s="12"/>
       <c r="B65" s="5">
         <v>4800</v>
       </c>
@@ -1783,11 +1789,11 @@
       <c r="E65" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="16.5">
-      <c r="A66" s="13"/>
-      <c r="B66" s="12">
+      <c r="A66" s="12"/>
+      <c r="B66" s="11">
         <v>9600</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C66" s="13">
         <v>3</v>
       </c>
       <c r="D66" s="4">
@@ -1796,7 +1802,7 @@
       <c r="E66" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="16.5">
-      <c r="A67" s="13"/>
+      <c r="A67" s="12"/>
       <c r="B67" s="5">
         <v>19200</v>
       </c>
@@ -1809,7 +1815,7 @@
       <c r="E67" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="16.5">
-      <c r="A68" s="13"/>
+      <c r="A68" s="12"/>
       <c r="B68" s="5">
         <v>57600</v>
       </c>
@@ -1822,7 +1828,7 @@
       <c r="E68" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="16.5">
-      <c r="A69" s="13"/>
+      <c r="A69" s="12"/>
       <c r="B69" s="5">
         <v>115200</v>
       </c>
@@ -1835,25 +1841,25 @@
       <c r="E69" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="16.5">
-      <c r="A70" s="13"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
       <c r="E70" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="16.5">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>79</v>
       </c>
       <c r="B71" s="5"/>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D71" s="13"/>
+      <c r="D71" s="12"/>
       <c r="E71" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="16.5">
-      <c r="A72" s="13"/>
+      <c r="A72" s="12"/>
       <c r="B72" s="5" t="s">
         <v>80</v>
       </c>
@@ -1863,12 +1869,12 @@
       <c r="D72" s="5">
         <v>150</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="16.5">
-      <c r="A73" s="13"/>
+      <c r="A73" s="12"/>
       <c r="B73" s="5" t="s">
         <v>83</v>
       </c>
@@ -1878,12 +1884,12 @@
       <c r="D73" s="5">
         <v>50</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="16.5">
-      <c r="A74" s="13"/>
+      <c r="A74" s="12"/>
       <c r="B74" s="5" t="s">
         <v>84</v>
       </c>
@@ -1893,12 +1899,12 @@
       <c r="D74" s="5">
         <v>90</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="16.5">
-      <c r="A75" s="13"/>
+      <c r="A75" s="12"/>
       <c r="B75" s="5" t="s">
         <v>86</v>
       </c>
@@ -1908,72 +1914,72 @@
       <c r="D75" s="5">
         <v>95</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="16.5">
-      <c r="A76" s="13"/>
+      <c r="A76" s="12"/>
       <c r="B76" s="5"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="13"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="16.5">
-      <c r="A77" s="13"/>
+      <c r="A77" s="12"/>
       <c r="B77" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C77" s="4">
         <v>1</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>88</v>
       </c>
       <c r="E77" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="16.5">
-      <c r="A78" s="13"/>
+      <c r="A78" s="12"/>
       <c r="B78" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C78" s="4">
         <v>2</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D78" s="12" t="s">
         <v>90</v>
       </c>
       <c r="E78" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="16.5">
-      <c r="A79" s="13"/>
+      <c r="A79" s="12"/>
       <c r="B79" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C79" s="4">
         <v>4</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>92</v>
       </c>
       <c r="E79" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="16.5">
-      <c r="A80" s="13"/>
+      <c r="A80" s="12"/>
       <c r="B80" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C80" s="4">
         <v>8</v>
       </c>
-      <c r="D80" s="13"/>
+      <c r="D80" s="12"/>
       <c r="E80" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="16.5">
-      <c r="A81" s="13"/>
+      <c r="A81" s="12"/>
       <c r="B81" s="5"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="13"/>
+      <c r="D81" s="12"/>
       <c r="E81" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="16.5">
@@ -1984,7 +1990,7 @@
       <c r="C82" s="4">
         <v>1</v>
       </c>
-      <c r="D82" s="13"/>
+      <c r="D82" s="12"/>
       <c r="E82" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="16.5">
@@ -1995,7 +2001,7 @@
       <c r="C83" s="4">
         <v>2</v>
       </c>
-      <c r="D83" s="13"/>
+      <c r="D83" s="12"/>
       <c r="E83" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="16.5">
@@ -2006,7 +2012,7 @@
       <c r="C84" s="4">
         <v>4</v>
       </c>
-      <c r="D84" s="13"/>
+      <c r="D84" s="12"/>
       <c r="E84" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="16.5">
@@ -2017,14 +2023,14 @@
       <c r="C85" s="4">
         <v>8</v>
       </c>
-      <c r="D85" s="13"/>
+      <c r="D85" s="12"/>
       <c r="E85" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="16.5">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="13"/>
+      <c r="D86" s="12"/>
       <c r="E86" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="16.5">
@@ -2035,7 +2041,7 @@
       <c r="C87" s="4">
         <v>1</v>
       </c>
-      <c r="D87" s="13"/>
+      <c r="D87" s="12"/>
       <c r="E87" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="16.5">
@@ -2046,133 +2052,133 @@
       <c r="C88" s="4">
         <v>2</v>
       </c>
-      <c r="D88" s="13"/>
+      <c r="D88" s="12"/>
       <c r="E88" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="16.5">
-      <c r="A89" s="13"/>
+      <c r="A89" s="12"/>
       <c r="B89" s="5"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
       <c r="E89" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="16.5">
       <c r="A90" s="3"/>
-      <c r="B90" s="10"/>
+      <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="16.5">
       <c r="A91" s="3"/>
-      <c r="B91" s="10"/>
+      <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="16.5">
-      <c r="A92" s="17" t="s">
+      <c r="A92" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B92" s="18"/>
+      <c r="B92" s="17"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="16.5">
-      <c r="A93" s="19" t="s">
+      <c r="A93" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B93" s="20"/>
+      <c r="B93" s="19"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="16.5">
-      <c r="A94" s="19"/>
-      <c r="B94" s="20"/>
+      <c r="A94" s="18"/>
+      <c r="B94" s="19"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="16.5">
-      <c r="A95" s="19"/>
-      <c r="B95" s="20"/>
+      <c r="A95" s="18"/>
+      <c r="B95" s="19"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="16.5">
-      <c r="A96" s="19" t="s">
+      <c r="A96" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B96" s="20"/>
+      <c r="B96" s="19"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="16.5">
-      <c r="A97" s="19"/>
-      <c r="B97" s="20"/>
+      <c r="A97" s="18"/>
+      <c r="B97" s="19"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="16.5">
-      <c r="A98" s="19" t="s">
+      <c r="A98" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B98" s="20"/>
+      <c r="B98" s="19"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="16.5">
-      <c r="A99" s="19" t="s">
+      <c r="A99" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="20"/>
+      <c r="B99" s="19"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="16.5">
-      <c r="A100" s="19"/>
-      <c r="B100" s="20"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="16.5">
-      <c r="A101" s="19" t="s">
+      <c r="A101" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B101" s="20"/>
+      <c r="B101" s="19"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="16.5">
-      <c r="A102" s="19"/>
-      <c r="B102" s="20"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="19"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="16.5">
-      <c r="A103" s="19" t="s">
+      <c r="A103" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B103" s="20"/>
+      <c r="B103" s="19"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="16.5">
-      <c r="A104" s="21" t="s">
+      <c r="A104" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="22"/>
+      <c r="B104" s="21"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>

</xml_diff>